<commit_message>
Dodalem prosty kalkulator funkcji brute force
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ThingsFromGithub\Studia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ThingsFromGithub\MDIAlgorytmicznie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B3E638-E107-4C74-9357-442B1E69CB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0882E7-ACB8-480C-84E9-BC6085DF599C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
   <si>
     <t>Spędzony czas</t>
   </si>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t>Tak naprawdę tylko na to przydało by się jeszcze z 5h</t>
+  </si>
+  <si>
+    <t>Jak starczy czasu</t>
+  </si>
+  <si>
+    <t>https://pl.khanacademy.org/math/differential-calculus/dc-chain#dc-chain-rule</t>
+  </si>
+  <si>
+    <t>https://pl.khanacademy.org/math/ap-calculus-ab/ab-diff-analytical-applications-new/ab-5-4/e/critical-numbers</t>
+  </si>
+  <si>
+    <t>Powt z ekstremów lok</t>
   </si>
 </sst>
 </file>
@@ -536,7 +548,7 @@
   <dimension ref="B4:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +834,9 @@
       <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="6"/>
+      <c r="E19" s="6">
+        <v>1.3</v>
+      </c>
       <c r="K19" t="s">
         <v>31</v>
       </c>
@@ -925,6 +939,12 @@
         <v>44440</v>
       </c>
       <c r="E29" s="6"/>
+      <c r="J29" t="s">
+        <v>54</v>
+      </c>
+      <c r="K29" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
@@ -934,6 +954,12 @@
         <v>20</v>
       </c>
       <c r="E30" s="6"/>
+      <c r="F30" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="1">

</xml_diff>